<commit_message>
co and push @ +
</commit_message>
<xml_diff>
--- a/Assets/Data/excel/功法数据表.xlsx
+++ b/Assets/Data/excel/功法数据表.xlsx
@@ -200,14 +200,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BaseSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BaseClever</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TgtPartGroup_Neck</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -661,6 +653,14 @@
   </si>
   <si>
     <t>#score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BaseCunning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BaseQuickness</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1377,7 +1377,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R24" sqref="R23:R24"/>
+      <selection pane="bottomRight" activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -1414,13 +1414,13 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K1" s="26"/>
       <c r="L1" s="26"/>
       <c r="M1" s="27"/>
       <c r="N1" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O1" s="26"/>
       <c r="P1" s="25" t="s">
@@ -1464,19 +1464,19 @@
     </row>
     <row r="2" spans="1:47" s="6" customFormat="1" ht="33" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
@@ -1488,25 +1488,25 @@
         <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>1</v>
@@ -1548,10 +1548,10 @@
         <v>12</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AD2" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AE2" s="26"/>
       <c r="AF2" s="26"/>
@@ -1559,7 +1559,7 @@
       <c r="AH2" s="26"/>
       <c r="AI2" s="27"/>
       <c r="AJ2" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AK2" s="5" t="s">
         <v>30</v>
@@ -1585,10 +1585,10 @@
     </row>
     <row r="3" spans="1:47" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -1638,112 +1638,112 @@
     </row>
     <row r="4" spans="1:47" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>36</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>41</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>40</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P4" s="14" t="s">
         <v>43</v>
       </c>
       <c r="Q4" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="S4" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="T4" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="R4" s="14" t="s">
+      <c r="U4" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="S4" s="14" t="s">
+      <c r="V4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="W4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="X4" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="T4" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="U4" s="14" t="s">
+      <c r="Y4" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="V4" s="14" t="s">
+      <c r="Z4" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA4" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="W4" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="X4" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y4" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z4" s="14" t="s">
+      <c r="AB4" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC4" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD4" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="AA4" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB4" s="14" t="s">
+      <c r="AE4" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="AC4" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="AD4" s="15" t="s">
+      <c r="AF4" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="AE4" s="15" t="s">
+      <c r="AG4" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH4" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="AF4" s="15" t="s">
+      <c r="AI4" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="AG4" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="AH4" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="AI4" s="15" t="s">
-        <v>66</v>
-      </c>
       <c r="AJ4" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AK4" s="14"/>
       <c r="AL4" s="14"/>
@@ -1759,19 +1759,19 @@
     </row>
     <row r="5" spans="1:47" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>37</v>
@@ -1783,88 +1783,88 @@
         <v>39</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>37</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L5" s="14" t="s">
         <v>37</v>
       </c>
       <c r="M5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="R5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="T5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="U5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="V5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="W5" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="N5" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="O5" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="P5" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q5" s="14" t="s">
+      <c r="X5" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="R5" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="S5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="T5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="U5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="V5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="W5" s="14" t="s">
+      <c r="Z5" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="X5" s="14" t="s">
+      <c r="AD5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG5" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ5" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="Y5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z5" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC5" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD5" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE5" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF5" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG5" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="AH5" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI5" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ5" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="AK5" s="14"/>
       <c r="AL5" s="14"/>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="6" spans="1:47" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -1980,7 +1980,7 @@
     </row>
     <row r="8" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -2032,16 +2032,16 @@
     <row r="9" spans="1:47" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18"/>
       <c r="B9" s="18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D9" s="18">
         <v>9</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F9" s="18">
         <v>5</v>
@@ -2060,11 +2060,11 @@
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
       <c r="M9" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N9" s="19"/>
       <c r="O9" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P9" s="19" t="s">
         <v>22</v>
@@ -2083,25 +2083,25 @@
       <c r="X9" s="19"/>
       <c r="Y9" s="19"/>
       <c r="Z9" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA9" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AB9" s="19"/>
       <c r="AC9" s="19"/>
       <c r="AD9" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AE9" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AF9" s="19"/>
       <c r="AG9" s="19"/>
       <c r="AH9" s="19"/>
       <c r="AI9" s="19"/>
       <c r="AJ9" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AK9" s="19"/>
       <c r="AL9" s="19"/>
@@ -2118,16 +2118,16 @@
     <row r="10" spans="1:47" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="18"/>
       <c r="B10" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D10" s="18">
         <v>8</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F10" s="18">
         <v>10</v>
@@ -2145,27 +2145,27 @@
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
       <c r="O10" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="P10" s="19" t="s">
         <v>26</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="S10" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T10" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="U10" s="19"/>
       <c r="V10" s="19"/>
@@ -2173,25 +2173,25 @@
       <c r="X10" s="19"/>
       <c r="Y10" s="19"/>
       <c r="Z10" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AA10" s="19"/>
       <c r="AB10" s="19"/>
       <c r="AC10" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AD10" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AE10" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AF10" s="19"/>
       <c r="AG10" s="19"/>
       <c r="AH10" s="19"/>
       <c r="AI10" s="19"/>
       <c r="AJ10" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AK10" s="19"/>
       <c r="AL10" s="19"/>
@@ -2208,16 +2208,16 @@
     <row r="11" spans="1:47" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="18"/>
       <c r="B11" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D11" s="18">
         <v>8</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F11" s="18">
         <v>10</v>
@@ -2235,12 +2235,12 @@
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
       <c r="L11" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
       <c r="O11" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="P11" s="19" t="s">
         <v>27</v>
@@ -2255,37 +2255,37 @@
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
       <c r="V11" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="W11" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="X11" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y11" s="19"/>
       <c r="Z11" s="19"/>
       <c r="AA11" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AB11" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AC11" s="19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AD11" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AE11" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AF11" s="19"/>
       <c r="AG11" s="19"/>
       <c r="AH11" s="19"/>
       <c r="AI11" s="19"/>
       <c r="AJ11" s="19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AK11" s="19"/>
       <c r="AL11" s="19"/>
@@ -2302,16 +2302,16 @@
     <row r="12" spans="1:47" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="18"/>
       <c r="B12" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D12" s="18">
         <v>8</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F12" s="18">
         <v>10</v>
@@ -2327,23 +2327,23 @@
         <v>100</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
       <c r="N12" s="19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O12" s="19"/>
       <c r="P12" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q12" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="R12" s="19" t="s">
         <v>118</v>
-      </c>
-      <c r="Q12" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="R12" s="19" t="s">
-        <v>120</v>
       </c>
       <c r="S12" s="19"/>
       <c r="T12" s="19"/>
@@ -2353,27 +2353,27 @@
       <c r="X12" s="19"/>
       <c r="Y12" s="19"/>
       <c r="Z12" s="19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="AA12" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB12" s="19" t="s">
         <v>128</v>
-      </c>
-      <c r="AB12" s="19" t="s">
-        <v>130</v>
       </c>
       <c r="AC12" s="19"/>
       <c r="AD12" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AE12" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AF12" s="19"/>
       <c r="AG12" s="19"/>
       <c r="AH12" s="19"/>
       <c r="AI12" s="19"/>
       <c r="AJ12" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AK12" s="19"/>
       <c r="AL12" s="19"/>
@@ -2390,16 +2390,16 @@
     <row r="13" spans="1:47" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="18"/>
       <c r="B13" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D13" s="18">
         <v>8</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F13" s="18">
         <v>10</v>
@@ -2415,21 +2415,21 @@
         <v>200</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
       <c r="M13" s="19"/>
       <c r="N13" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O13" s="19"/>
       <c r="P13" s="19"/>
       <c r="Q13" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R13" s="19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S13" s="19"/>
       <c r="T13" s="19"/>
@@ -2449,7 +2449,7 @@
       <c r="AH13" s="19"/>
       <c r="AI13" s="19"/>
       <c r="AJ13" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AK13" s="19"/>
       <c r="AL13" s="19"/>
@@ -2466,16 +2466,16 @@
     <row r="14" spans="1:47" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="18"/>
       <c r="B14" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D14" s="18">
         <v>8</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F14" s="18">
         <v>10</v>
@@ -2492,20 +2492,20 @@
       </c>
       <c r="J14" s="19"/>
       <c r="K14" s="19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
       <c r="N14" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="O14" s="19"/>
       <c r="P14" s="19"/>
       <c r="Q14" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R14" s="19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S14" s="19"/>
       <c r="T14" s="19"/>
@@ -2525,7 +2525,7 @@
       <c r="AH14" s="19"/>
       <c r="AI14" s="19"/>
       <c r="AJ14" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AK14" s="19"/>
       <c r="AL14" s="19"/>
@@ -2542,16 +2542,16 @@
     <row r="15" spans="1:47" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="18"/>
       <c r="B15" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D15" s="18">
         <v>8</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F15" s="18">
         <v>10</v>
@@ -2569,19 +2569,19 @@
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
       <c r="L15" s="19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
       <c r="O15" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P15" s="19"/>
       <c r="Q15" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R15" s="19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S15" s="19"/>
       <c r="T15" s="19"/>
@@ -2601,7 +2601,7 @@
       <c r="AH15" s="19"/>
       <c r="AI15" s="19"/>
       <c r="AJ15" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AK15" s="19"/>
       <c r="AL15" s="19"/>
@@ -2618,16 +2618,16 @@
     <row r="16" spans="1:47" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="18"/>
       <c r="B16" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D16" s="18">
         <v>8</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F16" s="18">
         <v>5</v>
@@ -2646,11 +2646,11 @@
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
       <c r="M16" s="19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N16" s="19"/>
       <c r="O16" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="P16" s="19"/>
       <c r="Q16" s="19" t="s">
@@ -2677,7 +2677,7 @@
       <c r="AH16" s="19"/>
       <c r="AI16" s="19"/>
       <c r="AJ16" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AK16" s="19"/>
       <c r="AL16" s="19"/>

</xml_diff>